<commit_message>
13.1-excel odd even making
</commit_message>
<xml_diff>
--- a/_static/_sample.xlsx
+++ b/_static/_sample.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="516" windowWidth="17568" windowHeight="7788"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>Python OpenPyXL module TEST</t>
   </si>
@@ -37,29 +38,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,22 +69,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -378,47 +366,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="17.296875" customWidth="1"/>
-    <col min="2" max="2" width="21.69921875" customWidth="1"/>
-    <col min="4" max="4" width="12.19921875" customWidth="1"/>
-    <col min="5" max="5" width="10.09765625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>43335.894001320623</v>
+      <c r="C1" s="1" t="n">
+        <v>43380.89074708818</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A2">
+    <row r="2" spans="1:5">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -436,8 +422,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>